<commit_message>
Reading, cleaning and plotting baseline data for simulation
</commit_message>
<xml_diff>
--- a/MyData.xlsx
+++ b/MyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentlit-my.sharepoint.com/personal/elaine_tynan_lit_ie/Documents/HDip/Semester2/ProgDataAnlys/repos/PfDA_Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{97864436-1BBF-498A-A9D6-819AE7E06A4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBB6A879-973F-48D1-9D7E-6A896FF4B23D}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{23D08EC2-E12C-48CE-B319-7B75B59D63AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8EF95F57-2E5B-419F-886E-0DB0DFA7A221}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="285" windowWidth="15375" windowHeight="14370" xr2:uid="{4E9EE3A0-650C-4A55-AEF7-713742751E40}"/>
+    <workbookView xWindow="34500" yWindow="180" windowWidth="13815" windowHeight="14370" xr2:uid="{4E9EE3A0-650C-4A55-AEF7-713742751E40}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="153">
   <si>
     <t>Course</t>
   </si>
@@ -59,12 +59,6 @@
     <t>IWD</t>
   </si>
   <si>
-    <t>Business Computing</t>
-  </si>
-  <si>
-    <t>Intro To Web Develpoment</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -80,54 +74,27 @@
     <t>RWD</t>
   </si>
   <si>
-    <t>Responsive Web Development</t>
-  </si>
-  <si>
     <t>DB1</t>
   </si>
   <si>
-    <t>DB</t>
-  </si>
-  <si>
-    <t>Databases 1</t>
-  </si>
-  <si>
     <t>PRG</t>
   </si>
   <si>
-    <t>Programming</t>
-  </si>
-  <si>
     <t>OSS</t>
   </si>
   <si>
-    <t>Operating Systems Structures</t>
-  </si>
-  <si>
     <t>CNSM</t>
   </si>
   <si>
-    <t>Computer Networks &amp; System Management</t>
-  </si>
-  <si>
     <t>ISD</t>
   </si>
   <si>
     <t>SD</t>
   </si>
   <si>
-    <t>Software Development</t>
-  </si>
-  <si>
-    <t>Internet Software Development</t>
-  </si>
-  <si>
     <t>RTES</t>
   </si>
   <si>
-    <t>Real Time Embedded Systems</t>
-  </si>
-  <si>
     <t>B7550</t>
   </si>
   <si>
@@ -525,6 +492,9 @@
   </si>
   <si>
     <t>C8793</t>
+  </si>
+  <si>
+    <t>Moodle Activity</t>
   </si>
 </sst>
 </file>
@@ -642,6 +612,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -941,10 +915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E4E9EB8-2BBF-4231-8CE2-75685A4692AA}">
-  <dimension ref="A1:N189"/>
+  <dimension ref="A1:J189"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,7 +931,7 @@
     <col min="9" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="6" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="6" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -965,19 +939,19 @@
         <v>3</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="E1" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>2</v>
@@ -985,8 +959,11 @@
       <c r="I1" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J1" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -1003,7 +980,7 @@
         <v>2021</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="H2" s="4">
         <v>0.66666666666666663</v>
@@ -1011,15 +988,11 @@
       <c r="I2" s="3">
         <v>93.4</v>
       </c>
-      <c r="J2" s="5"/>
-      <c r="M2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -1036,7 +1009,7 @@
         <v>2021</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="4">
@@ -1045,15 +1018,11 @@
       <c r="I3" s="3">
         <v>96.8</v>
       </c>
-      <c r="J3" s="5"/>
-      <c r="M3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -1070,7 +1039,7 @@
         <v>2021</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="4">
@@ -1079,15 +1048,11 @@
       <c r="I4" s="3">
         <v>39.799999999999997</v>
       </c>
-      <c r="J4" s="5"/>
-      <c r="M4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -1104,7 +1069,7 @@
         <v>2021</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="4">
@@ -1113,15 +1078,11 @@
       <c r="I5" s="3">
         <v>49.3</v>
       </c>
-      <c r="J5" s="5"/>
-      <c r="M5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -1138,15 +1099,17 @@
         <v>2021</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="4">
         <v>0</v>
       </c>
-      <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1163,21 +1126,15 @@
         <v>2021</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="4">
         <v>0</v>
       </c>
-      <c r="J7" s="5"/>
-      <c r="M7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J7"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
@@ -1194,7 +1151,7 @@
         <v>2021</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="4">
@@ -1203,15 +1160,11 @@
       <c r="I8" s="3">
         <v>59.7</v>
       </c>
-      <c r="J8" s="5"/>
-      <c r="M8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
@@ -1228,7 +1181,7 @@
         <v>2021</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="4">
@@ -1237,15 +1190,11 @@
       <c r="I9" s="3">
         <v>76.099999999999994</v>
       </c>
-      <c r="J9" s="5"/>
-      <c r="M9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
@@ -1262,7 +1211,7 @@
         <v>2021</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="4">
@@ -1271,15 +1220,11 @@
       <c r="I10" s="3">
         <v>51.3</v>
       </c>
-      <c r="J10" s="5"/>
-      <c r="M10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>5</v>
       </c>
@@ -1296,7 +1241,7 @@
         <v>2021</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="4">
@@ -1305,15 +1250,11 @@
       <c r="I11" s="3">
         <v>82.9</v>
       </c>
-      <c r="J11" s="5"/>
-      <c r="M11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>5</v>
       </c>
@@ -1330,7 +1271,7 @@
         <v>2021</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="4">
@@ -1339,15 +1280,11 @@
       <c r="I12" s="3">
         <v>53.4</v>
       </c>
-      <c r="J12" s="5"/>
-      <c r="M12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="N12" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>5</v>
       </c>
@@ -1364,7 +1301,7 @@
         <v>2021</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="4">
@@ -1373,9 +1310,11 @@
       <c r="I13" s="3">
         <v>61.010000000000005</v>
       </c>
-      <c r="J13" s="5"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>5</v>
       </c>
@@ -1392,7 +1331,7 @@
         <v>2021</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="4">
@@ -1401,9 +1340,11 @@
       <c r="I14" s="3">
         <v>4</v>
       </c>
-      <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>5</v>
       </c>
@@ -1420,7 +1361,7 @@
         <v>2021</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="4">
@@ -1429,9 +1370,11 @@
       <c r="I15" s="3">
         <v>68.849999999999994</v>
       </c>
-      <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>5</v>
       </c>
@@ -1448,7 +1391,7 @@
         <v>2021</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="4">
@@ -1457,7 +1400,9 @@
       <c r="I16" s="3">
         <v>80.3</v>
       </c>
-      <c r="J16" s="5"/>
+      <c r="J16">
+        <v>876</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
@@ -1476,7 +1421,7 @@
         <v>2021</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="4">
@@ -1485,7 +1430,9 @@
       <c r="I17" s="3">
         <v>15.79</v>
       </c>
-      <c r="J17" s="5"/>
+      <c r="J17">
+        <v>474</v>
+      </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
@@ -1504,7 +1451,7 @@
         <v>2021</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="4">
@@ -1513,7 +1460,9 @@
       <c r="I18" s="3">
         <v>1.98</v>
       </c>
-      <c r="J18" s="5"/>
+      <c r="J18">
+        <v>147</v>
+      </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
@@ -1532,7 +1481,7 @@
         <v>2021</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="4">
@@ -1541,7 +1490,9 @@
       <c r="I19" s="3">
         <v>6</v>
       </c>
-      <c r="J19" s="5"/>
+      <c r="J19">
+        <v>240</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
@@ -1560,7 +1511,7 @@
         <v>2021</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="4">
@@ -1569,7 +1520,9 @@
       <c r="I20" s="3">
         <v>1.6</v>
       </c>
-      <c r="J20" s="5"/>
+      <c r="J20">
+        <v>54</v>
+      </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
@@ -1588,7 +1541,7 @@
         <v>2021</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="4">
@@ -1597,7 +1550,9 @@
       <c r="I21" s="3">
         <v>63.7</v>
       </c>
-      <c r="J21" s="5"/>
+      <c r="J21">
+        <v>483</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -1616,7 +1571,7 @@
         <v>2021</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="4">
@@ -1625,7 +1580,9 @@
       <c r="I22" s="3">
         <v>78.2</v>
       </c>
-      <c r="J22" s="5"/>
+      <c r="J22">
+        <v>991</v>
+      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
@@ -1644,7 +1601,7 @@
         <v>2021</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="H23" s="4">
         <v>0.72222222222222221</v>
@@ -1652,14 +1609,16 @@
       <c r="I23" s="3">
         <v>63.05</v>
       </c>
-      <c r="J23" s="5"/>
+      <c r="J23">
+        <v>653</v>
+      </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C24" s="3">
         <v>1</v>
@@ -1671,7 +1630,7 @@
         <v>2021</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="4">
@@ -1680,14 +1639,16 @@
       <c r="I24" s="3">
         <v>66.38</v>
       </c>
-      <c r="J24" s="5"/>
+      <c r="J24">
+        <v>620</v>
+      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C25" s="3">
         <v>1</v>
@@ -1699,7 +1660,7 @@
         <v>2021</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="4">
@@ -1708,14 +1669,16 @@
       <c r="I25" s="3">
         <v>71.900000000000006</v>
       </c>
-      <c r="J25" s="5"/>
+      <c r="J25">
+        <v>441</v>
+      </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C26" s="3">
         <v>1</v>
@@ -1727,7 +1690,7 @@
         <v>2021</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="4">
@@ -1736,14 +1699,16 @@
       <c r="I26" s="3">
         <v>29.97</v>
       </c>
-      <c r="J26" s="5"/>
+      <c r="J26">
+        <v>1108</v>
+      </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C27" s="3">
         <v>1</v>
@@ -1755,7 +1720,7 @@
         <v>2021</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="4">
@@ -1764,14 +1729,16 @@
       <c r="I27" s="3">
         <v>0</v>
       </c>
-      <c r="J27" s="5"/>
+      <c r="J27">
+        <v>65</v>
+      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C28" s="3">
         <v>1</v>
@@ -1783,20 +1750,22 @@
         <v>2021</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="G28" s="1"/>
-      <c r="H28" s="4" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J28" s="5"/>
+      <c r="H28" s="4">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>2</v>
+      </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C29" s="3">
         <v>1</v>
@@ -1808,20 +1777,20 @@
         <v>2021</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="G29" s="1"/>
-      <c r="H29" s="4" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J29" s="5"/>
+      <c r="H29" s="4">
+        <v>0</v>
+      </c>
+      <c r="J29"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C30" s="3">
         <v>1</v>
@@ -1833,7 +1802,7 @@
         <v>2021</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="4">
@@ -1842,14 +1811,16 @@
       <c r="I30" s="3">
         <v>55.61</v>
       </c>
-      <c r="J30" s="5"/>
+      <c r="J30">
+        <v>875</v>
+      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C31" s="3">
         <v>1</v>
@@ -1861,7 +1832,7 @@
         <v>2021</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="4">
@@ -1870,14 +1841,16 @@
       <c r="I31" s="3">
         <v>0</v>
       </c>
-      <c r="J31" s="5"/>
+      <c r="J31">
+        <v>220</v>
+      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C32" s="3">
         <v>1</v>
@@ -1889,7 +1862,7 @@
         <v>2021</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="4">
@@ -1898,14 +1871,16 @@
       <c r="I32" s="3">
         <v>6.51</v>
       </c>
-      <c r="J32" s="5"/>
+      <c r="J32">
+        <v>555</v>
+      </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C33" s="3">
         <v>1</v>
@@ -1917,7 +1892,7 @@
         <v>2021</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="G33" s="1"/>
       <c r="H33" s="4">
@@ -1926,14 +1901,16 @@
       <c r="I33" s="3">
         <v>60.379999999999995</v>
       </c>
-      <c r="J33" s="5"/>
+      <c r="J33">
+        <v>684</v>
+      </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C34" s="3">
         <v>1</v>
@@ -1945,7 +1922,7 @@
         <v>2021</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="G34" s="1"/>
       <c r="H34" s="4">
@@ -1954,14 +1931,16 @@
       <c r="I34" s="3">
         <v>0</v>
       </c>
-      <c r="J34" s="5"/>
+      <c r="J34">
+        <v>60</v>
+      </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C35" s="3">
         <v>1</v>
@@ -1973,7 +1952,7 @@
         <v>2021</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="G35" s="1"/>
       <c r="H35" s="4">
@@ -1982,14 +1961,16 @@
       <c r="I35" s="3">
         <v>52.41</v>
       </c>
-      <c r="J35" s="5"/>
+      <c r="J35">
+        <v>1037</v>
+      </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C36" s="3">
         <v>1</v>
@@ -2001,20 +1982,20 @@
         <v>2021</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="G36" s="1"/>
       <c r="H36" s="4">
         <v>0</v>
       </c>
-      <c r="J36" s="5"/>
+      <c r="J36"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C37" s="3">
         <v>1</v>
@@ -2026,7 +2007,7 @@
         <v>2021</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="G37" s="1"/>
       <c r="H37" s="4">
@@ -2035,14 +2016,16 @@
       <c r="I37" s="3">
         <v>74.09</v>
       </c>
-      <c r="J37" s="5"/>
+      <c r="J37">
+        <v>966</v>
+      </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C38" s="3">
         <v>1</v>
@@ -2054,7 +2037,7 @@
         <v>2021</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="G38" s="1"/>
       <c r="H38" s="4">
@@ -2063,14 +2046,16 @@
       <c r="I38" s="3">
         <v>47.179999999999993</v>
       </c>
-      <c r="J38" s="5"/>
+      <c r="J38">
+        <v>913</v>
+      </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C39" s="3">
         <v>1</v>
@@ -2082,7 +2067,7 @@
         <v>2021</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="4">
@@ -2091,14 +2076,16 @@
       <c r="I39" s="3">
         <v>16.350000000000001</v>
       </c>
-      <c r="J39" s="5"/>
+      <c r="J39">
+        <v>574</v>
+      </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C40" s="3">
         <v>1</v>
@@ -2110,20 +2097,22 @@
         <v>2021</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G40" s="1"/>
-      <c r="H40" s="4" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J40" s="5"/>
+      <c r="H40" s="4">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>1</v>
+      </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C41" s="3">
         <v>1</v>
@@ -2135,20 +2124,20 @@
         <v>2021</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="G41" s="1"/>
       <c r="H41" s="4">
         <v>0</v>
       </c>
-      <c r="J41" s="5"/>
+      <c r="J41"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C42" s="3">
         <v>1</v>
@@ -2160,20 +2149,22 @@
         <v>2021</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="G42" s="1"/>
-      <c r="H42" s="4" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J42" s="5"/>
+      <c r="H42" s="4">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>1</v>
+      </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C43" s="3">
         <v>1</v>
@@ -2185,7 +2176,7 @@
         <v>2021</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="G43" s="1"/>
       <c r="H43" s="4">
@@ -2194,14 +2185,16 @@
       <c r="I43" s="3">
         <v>75.277999999999992</v>
       </c>
-      <c r="J43" s="5"/>
+      <c r="J43">
+        <v>453</v>
+      </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C44" s="3">
         <v>1</v>
@@ -2213,7 +2206,7 @@
         <v>2021</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="G44" s="2"/>
       <c r="H44" s="4">
@@ -2222,14 +2215,16 @@
       <c r="I44" s="3">
         <v>82.02</v>
       </c>
-      <c r="J44" s="5"/>
+      <c r="J44">
+        <v>681</v>
+      </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C45" s="3">
         <v>1</v>
@@ -2241,7 +2236,7 @@
         <v>2021</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="G45" s="2"/>
       <c r="H45" s="4">
@@ -2250,14 +2245,16 @@
       <c r="I45" s="3">
         <v>50.53</v>
       </c>
-      <c r="J45" s="5"/>
+      <c r="J45">
+        <v>445</v>
+      </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C46" s="3">
         <v>2</v>
@@ -2269,7 +2266,7 @@
         <v>2021</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="H46" s="4">
         <v>0.25</v>
@@ -2277,14 +2274,16 @@
       <c r="I46" s="3">
         <v>0</v>
       </c>
-      <c r="J46" s="5"/>
+      <c r="J46">
+        <v>31</v>
+      </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C47" s="3">
         <v>2</v>
@@ -2296,7 +2295,7 @@
         <v>2021</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="H47" s="4">
         <v>1</v>
@@ -2304,14 +2303,16 @@
       <c r="I47" s="3">
         <v>77.625</v>
       </c>
-      <c r="J47" s="5"/>
+      <c r="J47">
+        <v>503</v>
+      </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C48" s="3">
         <v>2</v>
@@ -2323,7 +2324,7 @@
         <v>2021</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="H48" s="4">
         <v>1</v>
@@ -2331,14 +2332,16 @@
       <c r="I48" s="3">
         <v>79.474999999999994</v>
       </c>
-      <c r="J48" s="5"/>
+      <c r="J48">
+        <v>236</v>
+      </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C49" s="3">
         <v>2</v>
@@ -2350,7 +2353,7 @@
         <v>2021</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="H49" s="4">
         <v>0.25</v>
@@ -2358,14 +2361,16 @@
       <c r="I49" s="3">
         <v>3.5</v>
       </c>
-      <c r="J49" s="5"/>
+      <c r="J49">
+        <v>105</v>
+      </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C50" s="3">
         <v>2</v>
@@ -2377,7 +2382,7 @@
         <v>2021</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="H50" s="4">
         <v>0.375</v>
@@ -2385,14 +2390,16 @@
       <c r="I50" s="3">
         <v>47.575000000000003</v>
       </c>
-      <c r="J50" s="5"/>
+      <c r="J50">
+        <v>217</v>
+      </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C51" s="3">
         <v>2</v>
@@ -2404,7 +2411,7 @@
         <v>2021</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="H51" s="4">
         <v>0.375</v>
@@ -2412,14 +2419,16 @@
       <c r="I51" s="3">
         <v>1.8250000000000002</v>
       </c>
-      <c r="J51" s="5"/>
+      <c r="J51">
+        <v>113</v>
+      </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C52" s="3">
         <v>2</v>
@@ -2431,7 +2440,7 @@
         <v>2021</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="H52" s="4">
         <v>0.88888888888888884</v>
@@ -2439,14 +2448,16 @@
       <c r="I52" s="3">
         <v>89.2</v>
       </c>
-      <c r="J52" s="5"/>
+      <c r="J52">
+        <v>227</v>
+      </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C53" s="3">
         <v>2</v>
@@ -2458,7 +2469,7 @@
         <v>2021</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="H53" s="4">
         <v>0.1111111111111111</v>
@@ -2466,14 +2477,16 @@
       <c r="I53" s="3">
         <v>60.399999999999991</v>
       </c>
-      <c r="J53" s="5"/>
+      <c r="J53">
+        <v>212</v>
+      </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C54" s="3">
         <v>2</v>
@@ -2485,7 +2498,7 @@
         <v>2021</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="H54" s="4">
         <v>1</v>
@@ -2493,14 +2506,16 @@
       <c r="I54" s="3">
         <v>91.05</v>
       </c>
-      <c r="J54" s="5"/>
+      <c r="J54">
+        <v>289</v>
+      </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C55" s="3">
         <v>2</v>
@@ -2512,22 +2527,22 @@
         <v>2021</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H55" s="4" t="e">
-        <v>#DIV/0!</v>
+        <v>50</v>
+      </c>
+      <c r="H55" s="4">
+        <v>0</v>
       </c>
       <c r="I55" s="3">
         <v>0</v>
       </c>
-      <c r="J55" s="5"/>
+      <c r="J55"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C56" s="3">
         <v>2</v>
@@ -2539,7 +2554,7 @@
         <v>2021</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="H56" s="4">
         <v>0</v>
@@ -2547,14 +2562,16 @@
       <c r="I56" s="3">
         <v>0</v>
       </c>
-      <c r="J56" s="5"/>
+      <c r="J56">
+        <v>43</v>
+      </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C57" s="3">
         <v>2</v>
@@ -2566,22 +2583,22 @@
         <v>2021</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H57" s="4" t="e">
-        <v>#DIV/0!</v>
+        <v>52</v>
+      </c>
+      <c r="H57" s="4">
+        <v>0</v>
       </c>
       <c r="I57" s="3">
         <v>0</v>
       </c>
-      <c r="J57" s="5"/>
+      <c r="J57"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C58" s="3">
         <v>2</v>
@@ -2593,7 +2610,7 @@
         <v>2021</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="H58" s="4">
         <v>0</v>
@@ -2601,14 +2618,16 @@
       <c r="I58" s="3">
         <v>1.25</v>
       </c>
-      <c r="J58" s="5"/>
+      <c r="J58">
+        <v>224</v>
+      </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C59" s="3">
         <v>2</v>
@@ -2620,22 +2639,22 @@
         <v>2021</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H59" s="4" t="e">
-        <v>#DIV/0!</v>
+        <v>54</v>
+      </c>
+      <c r="H59" s="4">
+        <v>0</v>
       </c>
       <c r="I59" s="3">
         <v>0</v>
       </c>
-      <c r="J59" s="5"/>
+      <c r="J59"/>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C60" s="3">
         <v>2</v>
@@ -2647,7 +2666,7 @@
         <v>2021</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="H60" s="4">
         <v>0.25</v>
@@ -2655,14 +2674,16 @@
       <c r="I60" s="3">
         <v>26.5</v>
       </c>
-      <c r="J60" s="5"/>
+      <c r="J60">
+        <v>227</v>
+      </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C61" s="3">
         <v>1</v>
@@ -2674,7 +2695,7 @@
         <v>2020</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="H61" s="4">
         <v>1</v>
@@ -2689,7 +2710,7 @@
         <v>5</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C62" s="3">
         <v>1</v>
@@ -2701,7 +2722,7 @@
         <v>2020</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="H62" s="4">
         <v>1</v>
@@ -2716,7 +2737,7 @@
         <v>5</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C63" s="3">
         <v>1</v>
@@ -2728,7 +2749,7 @@
         <v>2020</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="H63" s="4">
         <v>1</v>
@@ -2743,7 +2764,7 @@
         <v>5</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C64" s="3">
         <v>1</v>
@@ -2755,7 +2776,7 @@
         <v>2020</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="H64" s="4">
         <v>1</v>
@@ -2770,7 +2791,7 @@
         <v>5</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C65" s="3">
         <v>1</v>
@@ -2782,7 +2803,7 @@
         <v>2020</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="H65" s="4">
         <v>1</v>
@@ -2797,7 +2818,7 @@
         <v>5</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C66" s="3">
         <v>1</v>
@@ -2809,7 +2830,7 @@
         <v>2020</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="H66" s="4">
         <v>1</v>
@@ -2824,7 +2845,7 @@
         <v>5</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C67" s="3">
         <v>1</v>
@@ -2836,7 +2857,7 @@
         <v>2020</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="H67" s="4">
         <v>0.8</v>
@@ -2851,7 +2872,7 @@
         <v>5</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C68" s="3">
         <v>1</v>
@@ -2863,7 +2884,7 @@
         <v>2020</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="H68" s="4">
         <v>1</v>
@@ -2878,7 +2899,7 @@
         <v>5</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C69" s="3">
         <v>1</v>
@@ -2890,7 +2911,7 @@
         <v>2020</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="H69" s="4">
         <v>1</v>
@@ -2905,7 +2926,7 @@
         <v>5</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C70" s="3">
         <v>1</v>
@@ -2917,7 +2938,7 @@
         <v>2020</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="H70" s="4">
         <v>0.6</v>
@@ -2932,7 +2953,7 @@
         <v>5</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C71" s="3">
         <v>1</v>
@@ -2944,7 +2965,7 @@
         <v>2020</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="H71" s="4">
         <v>0.8</v>
@@ -2959,7 +2980,7 @@
         <v>5</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C72" s="3">
         <v>1</v>
@@ -2971,7 +2992,7 @@
         <v>2020</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="H72" s="4">
         <v>0.4</v>
@@ -2986,7 +3007,7 @@
         <v>5</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C73" s="3">
         <v>1</v>
@@ -2998,7 +3019,7 @@
         <v>2020</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="H73" s="4">
         <v>1</v>
@@ -3013,7 +3034,7 @@
         <v>5</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C74" s="3">
         <v>1</v>
@@ -3025,7 +3046,7 @@
         <v>2020</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="H74" s="4">
         <v>0.8</v>
@@ -3040,7 +3061,7 @@
         <v>5</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C75" s="3">
         <v>1</v>
@@ -3052,7 +3073,7 @@
         <v>2020</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="H75" s="4">
         <v>0.6</v>
@@ -3067,7 +3088,7 @@
         <v>5</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C76" s="3">
         <v>1</v>
@@ -3079,7 +3100,7 @@
         <v>2020</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="H76" s="4">
         <v>0.8</v>
@@ -3094,7 +3115,7 @@
         <v>5</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C77" s="3">
         <v>1</v>
@@ -3106,7 +3127,7 @@
         <v>2020</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="H77" s="4">
         <v>0.6</v>
@@ -3121,7 +3142,7 @@
         <v>5</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C78" s="3">
         <v>1</v>
@@ -3133,7 +3154,7 @@
         <v>2020</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="H78" s="4">
         <v>0.53846153846153844</v>
@@ -3148,7 +3169,7 @@
         <v>5</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C79" s="3">
         <v>1</v>
@@ -3160,7 +3181,7 @@
         <v>2020</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="H79" s="4">
         <v>0.88461538461538458</v>
@@ -3175,7 +3196,7 @@
         <v>5</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C80" s="3">
         <v>1</v>
@@ -3187,7 +3208,7 @@
         <v>2020</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="H80" s="4">
         <v>0.96153846153846156</v>
@@ -3202,7 +3223,7 @@
         <v>5</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C81" s="3">
         <v>1</v>
@@ -3214,7 +3235,7 @@
         <v>2020</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="H81" s="4">
         <v>0.84615384615384615</v>
@@ -3229,7 +3250,7 @@
         <v>5</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C82" s="3">
         <v>1</v>
@@ -3241,7 +3262,7 @@
         <v>2020</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="H82" s="4">
         <v>0.84615384615384615</v>
@@ -3256,7 +3277,7 @@
         <v>5</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C83" s="3">
         <v>1</v>
@@ -3268,7 +3289,7 @@
         <v>2020</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="H83" s="4">
         <v>0.92307692307692313</v>
@@ -3283,7 +3304,7 @@
         <v>5</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C84" s="3">
         <v>1</v>
@@ -3295,7 +3316,7 @@
         <v>2020</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="H84" s="4">
         <v>0.96153846153846156</v>
@@ -3310,7 +3331,7 @@
         <v>5</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C85" s="3">
         <v>1</v>
@@ -3322,7 +3343,7 @@
         <v>2020</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="H85" s="4">
         <v>0.88461538461538458</v>
@@ -3337,7 +3358,7 @@
         <v>5</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C86" s="3">
         <v>1</v>
@@ -3349,7 +3370,7 @@
         <v>2020</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="H86" s="4">
         <v>0.84615384615384615</v>
@@ -3364,7 +3385,7 @@
         <v>5</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C87" s="3">
         <v>1</v>
@@ -3376,7 +3397,7 @@
         <v>2020</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="H87" s="4">
         <v>0.82692307692307687</v>
@@ -3391,7 +3412,7 @@
         <v>5</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C88" s="3">
         <v>1</v>
@@ -3403,7 +3424,7 @@
         <v>2020</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="H88" s="4">
         <v>0.54</v>
@@ -3418,7 +3439,7 @@
         <v>5</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C89" s="3">
         <v>1</v>
@@ -3430,7 +3451,7 @@
         <v>2020</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="H89" s="4">
         <v>0.73076923076923073</v>
@@ -3445,7 +3466,7 @@
         <v>5</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C90" s="3">
         <v>1</v>
@@ -3457,7 +3478,7 @@
         <v>2020</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="H90" s="4">
         <v>0.75</v>
@@ -3472,7 +3493,7 @@
         <v>5</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C91" s="3">
         <v>1</v>
@@ -3484,7 +3505,7 @@
         <v>2020</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="H91" s="4">
         <v>1</v>
@@ -3499,7 +3520,7 @@
         <v>5</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C92" s="3">
         <v>1</v>
@@ -3511,7 +3532,7 @@
         <v>2020</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="H92" s="4">
         <v>0.61538461538461542</v>
@@ -3526,7 +3547,7 @@
         <v>5</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C93" s="3">
         <v>1</v>
@@ -3538,7 +3559,7 @@
         <v>2020</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="H93" s="4">
         <v>0.21428571428571427</v>
@@ -3550,7 +3571,7 @@
         <v>5</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C94" s="3">
         <v>1</v>
@@ -3562,7 +3583,7 @@
         <v>2020</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="H94" s="4">
         <v>0.54</v>
@@ -3577,7 +3598,7 @@
         <v>5</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C95" s="3">
         <v>1</v>
@@ -3589,7 +3610,7 @@
         <v>2020</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="H95" s="4">
         <v>0.61538461538461542</v>
@@ -3604,7 +3625,7 @@
         <v>5</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C96" s="3">
         <v>1</v>
@@ -3616,7 +3637,7 @@
         <v>2020</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="H96" s="4">
         <v>0.9</v>
@@ -3631,7 +3652,7 @@
         <v>5</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C97" s="3">
         <v>1</v>
@@ -3643,7 +3664,7 @@
         <v>2020</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="H97" s="4">
         <v>0.21052631578947367</v>
@@ -3658,7 +3679,7 @@
         <v>5</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C98" s="3">
         <v>1</v>
@@ -3670,7 +3691,7 @@
         <v>2020</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="H98" s="4">
         <v>0.76</v>
@@ -3685,7 +3706,7 @@
         <v>5</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C99" s="3">
         <v>1</v>
@@ -3697,7 +3718,7 @@
         <v>2020</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="H99" s="4">
         <v>0.8</v>
@@ -3712,7 +3733,7 @@
         <v>5</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C100" s="3">
         <v>1</v>
@@ -3724,7 +3745,7 @@
         <v>2020</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="H100" s="4">
         <v>0.96</v>
@@ -3739,7 +3760,7 @@
         <v>5</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C101" s="3">
         <v>1</v>
@@ -3751,7 +3772,7 @@
         <v>2020</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="H101" s="4" t="e">
         <v>#DIV/0!</v>
@@ -3763,7 +3784,7 @@
         <v>5</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C102" s="3">
         <v>1</v>
@@ -3775,7 +3796,7 @@
         <v>2020</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="H102" s="4">
         <v>1</v>
@@ -3790,7 +3811,7 @@
         <v>5</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C103" s="3">
         <v>1</v>
@@ -3802,7 +3823,7 @@
         <v>2020</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="H103" s="4">
         <v>0.72</v>
@@ -3817,7 +3838,7 @@
         <v>5</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C104" s="3">
         <v>1</v>
@@ -3829,7 +3850,7 @@
         <v>2020</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="H104" s="4">
         <v>0.28000000000000003</v>
@@ -3844,7 +3865,7 @@
         <v>5</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C105" s="3">
         <v>1</v>
@@ -3856,7 +3877,7 @@
         <v>2020</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="H105" s="4">
         <v>0.84</v>
@@ -3871,7 +3892,7 @@
         <v>5</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C106" s="3">
         <v>1</v>
@@ -3883,7 +3904,7 @@
         <v>2020</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="H106" s="4">
         <v>0.28000000000000003</v>
@@ -3898,7 +3919,7 @@
         <v>5</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C107" s="3">
         <v>1</v>
@@ -3910,7 +3931,7 @@
         <v>2020</v>
       </c>
       <c r="F107" s="3" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="H107" s="4">
         <v>0.6</v>
@@ -3925,7 +3946,7 @@
         <v>5</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C108" s="3">
         <v>1</v>
@@ -3937,7 +3958,7 @@
         <v>2020</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="H108" s="4">
         <v>0.24</v>
@@ -3952,7 +3973,7 @@
         <v>5</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C109" s="3">
         <v>1</v>
@@ -3964,7 +3985,7 @@
         <v>2020</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="H109" s="4" t="e">
         <v>#DIV/0!</v>
@@ -3979,7 +4000,7 @@
         <v>5</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C110" s="3">
         <v>1</v>
@@ -3991,7 +4012,7 @@
         <v>2020</v>
       </c>
       <c r="F110" s="3" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="H110" s="4">
         <v>0.88</v>
@@ -4003,10 +4024,10 @@
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C111" s="3">
         <v>2</v>
@@ -4018,7 +4039,7 @@
         <v>2019</v>
       </c>
       <c r="F111" s="3" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="H111" s="4">
         <v>1</v>
@@ -4030,10 +4051,10 @@
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C112" s="3">
         <v>2</v>
@@ -4045,7 +4066,7 @@
         <v>2019</v>
       </c>
       <c r="F112" s="3" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="H112" s="4">
         <v>0.52380952380952384</v>
@@ -4057,10 +4078,10 @@
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C113" s="3">
         <v>2</v>
@@ -4072,7 +4093,7 @@
         <v>2019</v>
       </c>
       <c r="F113" s="3" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="H113" s="4">
         <v>0.23809523809523808</v>
@@ -4084,10 +4105,10 @@
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C114" s="3">
         <v>2</v>
@@ -4099,7 +4120,7 @@
         <v>2019</v>
       </c>
       <c r="F114" s="3" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="H114" s="4">
         <v>0.52380952380952384</v>
@@ -4111,10 +4132,10 @@
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C115" s="3">
         <v>2</v>
@@ -4126,7 +4147,7 @@
         <v>2019</v>
       </c>
       <c r="F115" s="3" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="H115" s="4">
         <v>0.80952380952380953</v>
@@ -4138,10 +4159,10 @@
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C116" s="3">
         <v>2</v>
@@ -4153,7 +4174,7 @@
         <v>2019</v>
       </c>
       <c r="F116" s="3" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="H116" s="4">
         <v>0.76190476190476186</v>
@@ -4165,10 +4186,10 @@
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C117" s="3">
         <v>2</v>
@@ -4180,7 +4201,7 @@
         <v>2019</v>
       </c>
       <c r="F117" s="3" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H117" s="4">
         <v>0.80952380952380953</v>
@@ -4192,10 +4213,10 @@
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C118" s="3">
         <v>2</v>
@@ -4207,7 +4228,7 @@
         <v>2019</v>
       </c>
       <c r="F118" s="3" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="H118" s="4">
         <v>1</v>
@@ -4219,10 +4240,10 @@
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C119" s="3">
         <v>2</v>
@@ -4234,7 +4255,7 @@
         <v>2019</v>
       </c>
       <c r="F119" s="3" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H119" s="4">
         <v>1</v>
@@ -4246,10 +4267,10 @@
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C120" s="3">
         <v>2</v>
@@ -4261,7 +4282,7 @@
         <v>2019</v>
       </c>
       <c r="F120" s="3" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="H120" s="4">
         <v>0.80952380952380953</v>
@@ -4273,10 +4294,10 @@
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C121" s="3">
         <v>2</v>
@@ -4288,7 +4309,7 @@
         <v>2019</v>
       </c>
       <c r="F121" s="3" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="H121" s="4">
         <v>1</v>
@@ -4300,10 +4321,10 @@
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C122" s="3">
         <v>2</v>
@@ -4315,7 +4336,7 @@
         <v>2019</v>
       </c>
       <c r="F122" s="3" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="H122" s="4">
         <v>0.7142857142857143</v>
@@ -4327,10 +4348,10 @@
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C123" s="3">
         <v>2</v>
@@ -4342,7 +4363,7 @@
         <v>2019</v>
       </c>
       <c r="F123" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="H123" s="4">
         <v>0.90476190476190477</v>
@@ -4354,10 +4375,10 @@
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C124" s="3">
         <v>2</v>
@@ -4369,7 +4390,7 @@
         <v>2019</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="H124" s="4">
         <v>0.8571428571428571</v>
@@ -4381,10 +4402,10 @@
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C125" s="3">
         <v>2</v>
@@ -4396,7 +4417,7 @@
         <v>2019</v>
       </c>
       <c r="F125" s="3" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="H125" s="4">
         <v>0.90476190476190477</v>
@@ -4408,10 +4429,10 @@
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C126" s="3">
         <v>2</v>
@@ -4423,7 +4444,7 @@
         <v>2019</v>
       </c>
       <c r="F126" s="3" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="H126" s="4">
         <v>0.7142857142857143</v>
@@ -4435,10 +4456,10 @@
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C127" s="3">
         <v>2</v>
@@ -4450,7 +4471,7 @@
         <v>2019</v>
       </c>
       <c r="F127" s="3" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="H127" s="4">
         <v>0.33333333333333331</v>
@@ -4462,10 +4483,10 @@
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C128" s="3">
         <v>2</v>
@@ -4477,7 +4498,7 @@
         <v>2019</v>
       </c>
       <c r="F128" s="3" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="H128" s="4">
         <v>0.95238095238095233</v>
@@ -4489,10 +4510,10 @@
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C129" s="3">
         <v>2</v>
@@ -4504,7 +4525,7 @@
         <v>2019</v>
       </c>
       <c r="F129" s="3" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="H129" s="4">
         <v>0.23809523809523808</v>
@@ -4516,10 +4537,10 @@
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C130" s="3">
         <v>2</v>
@@ -4531,7 +4552,7 @@
         <v>2019</v>
       </c>
       <c r="F130" s="3" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="H130" s="4">
         <v>0.7142857142857143</v>
@@ -4543,10 +4564,10 @@
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C131" s="3">
         <v>2</v>
@@ -4558,7 +4579,7 @@
         <v>2019</v>
       </c>
       <c r="F131" s="3" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="H131" s="4">
         <v>0.61904761904761907</v>
@@ -4570,10 +4591,10 @@
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C132" s="3">
         <v>2</v>
@@ -4585,7 +4606,7 @@
         <v>2019</v>
       </c>
       <c r="F132" s="3" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="H132" s="4">
         <v>0.42857142857142855</v>
@@ -4597,10 +4618,10 @@
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C133" s="3">
         <v>3</v>
@@ -4612,7 +4633,7 @@
         <v>2019</v>
       </c>
       <c r="F133" s="3" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="H133" s="4">
         <v>0.5</v>
@@ -4624,10 +4645,10 @@
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C134" s="3">
         <v>3</v>
@@ -4639,7 +4660,7 @@
         <v>2019</v>
       </c>
       <c r="F134" s="3" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="H134" s="4">
         <v>0.25</v>
@@ -4651,10 +4672,10 @@
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C135" s="3">
         <v>3</v>
@@ -4666,7 +4687,7 @@
         <v>2019</v>
       </c>
       <c r="F135" s="3" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="H135" s="4">
         <v>0.9642857142857143</v>
@@ -4678,10 +4699,10 @@
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C136" s="3">
         <v>3</v>
@@ -4693,7 +4714,7 @@
         <v>2019</v>
       </c>
       <c r="F136" s="3" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="H136" s="4">
         <v>0.8928571428571429</v>
@@ -4705,10 +4726,10 @@
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C137" s="3">
         <v>3</v>
@@ -4720,7 +4741,7 @@
         <v>2019</v>
       </c>
       <c r="F137" s="3" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="H137" s="4">
         <v>0.7857142857142857</v>
@@ -4732,10 +4753,10 @@
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C138" s="3">
         <v>3</v>
@@ -4747,7 +4768,7 @@
         <v>2019</v>
       </c>
       <c r="F138" s="3" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="H138" s="4">
         <v>0</v>
@@ -4759,10 +4780,10 @@
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C139" s="3">
         <v>3</v>
@@ -4774,7 +4795,7 @@
         <v>2019</v>
       </c>
       <c r="F139" s="3" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="H139" s="4">
         <v>0.5714285714285714</v>
@@ -4786,10 +4807,10 @@
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C140" s="3">
         <v>3</v>
@@ -4801,7 +4822,7 @@
         <v>2019</v>
       </c>
       <c r="F140" s="3" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="H140" s="4">
         <v>1</v>
@@ -4813,10 +4834,10 @@
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C141" s="3">
         <v>3</v>
@@ -4828,7 +4849,7 @@
         <v>2019</v>
       </c>
       <c r="F141" s="3" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="H141" s="4">
         <v>0.79285714285714282</v>
@@ -4840,10 +4861,10 @@
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C142" s="3">
         <v>3</v>
@@ -4855,7 +4876,7 @@
         <v>2019</v>
       </c>
       <c r="F142" s="3" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="H142" s="4">
         <v>0.8928571428571429</v>
@@ -4867,10 +4888,10 @@
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C143" s="3">
         <v>3</v>
@@ -4882,7 +4903,7 @@
         <v>2019</v>
       </c>
       <c r="F143" s="3" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="H143" s="4">
         <v>1</v>
@@ -4894,10 +4915,10 @@
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C144" s="3">
         <v>3</v>
@@ -4909,7 +4930,7 @@
         <v>2019</v>
       </c>
       <c r="F144" s="3" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="H144" s="4">
         <v>0.9642857142857143</v>
@@ -4921,10 +4942,10 @@
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C145" s="3">
         <v>3</v>
@@ -4936,7 +4957,7 @@
         <v>2019</v>
       </c>
       <c r="F145" s="3" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="H145" s="4">
         <v>0.5</v>
@@ -4948,10 +4969,10 @@
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C146" s="3">
         <v>3</v>
@@ -4963,7 +4984,7 @@
         <v>2019</v>
       </c>
       <c r="F146" s="3" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="H146" s="4">
         <v>0.6071428571428571</v>
@@ -4975,10 +4996,10 @@
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C147" s="3">
         <v>3</v>
@@ -4990,7 +5011,7 @@
         <v>2019</v>
       </c>
       <c r="F147" s="3" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="H147" s="4">
         <v>0.75</v>
@@ -5002,10 +5023,10 @@
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C148" s="3">
         <v>3</v>
@@ -5017,7 +5038,7 @@
         <v>2019</v>
       </c>
       <c r="F148" s="3" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="H148" s="4">
         <v>1</v>
@@ -5029,10 +5050,10 @@
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C149" s="3">
         <v>3</v>
@@ -5044,7 +5065,7 @@
         <v>2019</v>
       </c>
       <c r="F149" s="3" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="H149" s="4">
         <v>0.42857142857142855</v>
@@ -5056,10 +5077,10 @@
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C150" s="3">
         <v>3</v>
@@ -5071,7 +5092,7 @@
         <v>2019</v>
       </c>
       <c r="F150" s="3" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="H150" s="4">
         <v>0.89655172413793105</v>
@@ -5083,10 +5104,10 @@
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C151" s="3">
         <v>3</v>
@@ -5098,7 +5119,7 @@
         <v>2019</v>
       </c>
       <c r="F151" s="3" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="H151" s="4">
         <v>0.48275862068965519</v>
@@ -5110,10 +5131,10 @@
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C152" s="3">
         <v>3</v>
@@ -5125,7 +5146,7 @@
         <v>2019</v>
       </c>
       <c r="F152" s="3" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="H152" s="4">
         <v>0.75862068965517238</v>
@@ -5137,10 +5158,10 @@
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C153" s="3">
         <v>3</v>
@@ -5152,7 +5173,7 @@
         <v>2019</v>
       </c>
       <c r="F153" s="3" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="H153" s="4">
         <v>0.72413793103448276</v>
@@ -5164,10 +5185,10 @@
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C154" s="3">
         <v>3</v>
@@ -5179,7 +5200,7 @@
         <v>2019</v>
       </c>
       <c r="F154" s="3" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="H154" s="4">
         <v>0.58620689655172409</v>
@@ -5191,10 +5212,10 @@
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C155" s="3">
         <v>3</v>
@@ -5206,7 +5227,7 @@
         <v>2019</v>
       </c>
       <c r="F155" s="3" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="H155" s="4">
         <v>0.58620689655172409</v>
@@ -5218,10 +5239,10 @@
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C156" s="3">
         <v>3</v>
@@ -5233,7 +5254,7 @@
         <v>2019</v>
       </c>
       <c r="F156" s="3" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="H156" s="4">
         <v>0.7931034482758621</v>
@@ -5245,10 +5266,10 @@
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C157" s="3">
         <v>3</v>
@@ -5260,7 +5281,7 @@
         <v>2019</v>
       </c>
       <c r="F157" s="3" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="H157" s="4">
         <v>0.55172413793103448</v>
@@ -5272,10 +5293,10 @@
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C158" s="3">
         <v>3</v>
@@ -5287,7 +5308,7 @@
         <v>2019</v>
       </c>
       <c r="F158" s="3" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="H158" s="4">
         <v>0.62068965517241381</v>
@@ -5299,10 +5320,10 @@
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C159" s="3">
         <v>3</v>
@@ -5314,7 +5335,7 @@
         <v>2019</v>
       </c>
       <c r="F159" s="3" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="H159" s="4">
         <v>0.75862068965517238</v>
@@ -5326,10 +5347,10 @@
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C160" s="3">
         <v>3</v>
@@ -5341,7 +5362,7 @@
         <v>2019</v>
       </c>
       <c r="F160" s="3" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="H160" s="4">
         <v>0.82758620689655171</v>
@@ -5353,10 +5374,10 @@
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C161" s="3">
         <v>3</v>
@@ -5368,7 +5389,7 @@
         <v>2019</v>
       </c>
       <c r="F161" s="3" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="H161" s="4">
         <v>0.72413793103448276</v>
@@ -5380,10 +5401,10 @@
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C162" s="3">
         <v>3</v>
@@ -5395,7 +5416,7 @@
         <v>2019</v>
       </c>
       <c r="F162" s="3" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="H162" s="4">
         <v>0.7931034482758621</v>
@@ -5407,10 +5428,10 @@
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C163" s="3">
         <v>3</v>
@@ -5422,7 +5443,7 @@
         <v>2019</v>
       </c>
       <c r="F163" s="3" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="H163" s="4">
         <v>0.37931034482758619</v>
@@ -5434,10 +5455,10 @@
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C164" s="3">
         <v>3</v>
@@ -5449,7 +5470,7 @@
         <v>2019</v>
       </c>
       <c r="F164" s="3" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="H164" s="4">
         <v>0.2413793103448276</v>
@@ -5461,10 +5482,10 @@
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C165" s="3">
         <v>3</v>
@@ -5476,7 +5497,7 @@
         <v>2019</v>
       </c>
       <c r="F165" s="3" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="H165" s="4">
         <v>0.93103448275862066</v>
@@ -5488,10 +5509,10 @@
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C166" s="3">
         <v>3</v>
@@ -5503,7 +5524,7 @@
         <v>2019</v>
       </c>
       <c r="F166" s="3" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="H166" s="4">
         <v>0.75862068965517238</v>
@@ -5515,10 +5536,10 @@
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C167" s="3">
         <v>3</v>
@@ -5530,7 +5551,7 @@
         <v>2019</v>
       </c>
       <c r="F167" s="3" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="H167" s="4">
         <v>0.89655172413793105</v>
@@ -5542,10 +5563,10 @@
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C168" s="3">
         <v>3</v>
@@ -5557,7 +5578,7 @@
         <v>2019</v>
       </c>
       <c r="F168" s="3" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="H168" s="4">
         <v>0.93103448275862066</v>
@@ -5569,10 +5590,10 @@
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C169" s="3">
         <v>3</v>
@@ -5584,7 +5605,7 @@
         <v>2019</v>
       </c>
       <c r="F169" s="3" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="H169" s="4">
         <v>0.4</v>
@@ -5596,10 +5617,10 @@
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C170" s="3">
         <v>3</v>
@@ -5611,7 +5632,7 @@
         <v>2019</v>
       </c>
       <c r="F170" s="3" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="H170" s="4">
         <v>0.38333333333333336</v>
@@ -5623,10 +5644,10 @@
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C171" s="3">
         <v>3</v>
@@ -5638,7 +5659,7 @@
         <v>2019</v>
       </c>
       <c r="F171" s="3" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="H171" s="4">
         <v>0</v>
@@ -5650,10 +5671,10 @@
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C172" s="3">
         <v>3</v>
@@ -5665,7 +5686,7 @@
         <v>2019</v>
       </c>
       <c r="F172" s="3" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="H172" s="4">
         <v>0.66666666666666663</v>
@@ -5677,10 +5698,10 @@
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C173" s="3">
         <v>3</v>
@@ -5692,7 +5713,7 @@
         <v>2019</v>
       </c>
       <c r="F173" s="3" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="H173" s="4">
         <v>0.5</v>
@@ -5704,10 +5725,10 @@
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C174" s="3">
         <v>3</v>
@@ -5719,7 +5740,7 @@
         <v>2019</v>
       </c>
       <c r="F174" s="3" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="H174" s="4">
         <v>0.36666666666666664</v>
@@ -5731,10 +5752,10 @@
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C175" s="3">
         <v>3</v>
@@ -5746,7 +5767,7 @@
         <v>2019</v>
       </c>
       <c r="F175" s="3" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="H175" s="4">
         <v>0.6333333333333333</v>
@@ -5758,10 +5779,10 @@
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C176" s="3">
         <v>3</v>
@@ -5773,7 +5794,7 @@
         <v>2019</v>
       </c>
       <c r="F176" s="3" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="H176" s="4">
         <v>0.6</v>
@@ -5785,10 +5806,10 @@
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C177" s="3">
         <v>3</v>
@@ -5800,7 +5821,7 @@
         <v>2019</v>
       </c>
       <c r="F177" s="3" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="H177" s="4">
         <v>0.43333333333333335</v>
@@ -5812,10 +5833,10 @@
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C178" s="3">
         <v>3</v>
@@ -5827,7 +5848,7 @@
         <v>2019</v>
       </c>
       <c r="F178" s="3" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="H178" s="4">
         <v>3.3333333333333333E-2</v>
@@ -5839,10 +5860,10 @@
     </row>
     <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C179" s="3">
         <v>3</v>
@@ -5854,7 +5875,7 @@
         <v>2019</v>
       </c>
       <c r="F179" s="3" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="H179" s="4">
         <v>0.77419354838709675</v>
@@ -5866,10 +5887,10 @@
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C180" s="3">
         <v>3</v>
@@ -5881,7 +5902,7 @@
         <v>2019</v>
       </c>
       <c r="F180" s="3" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="H180" s="4">
         <v>0.3</v>
@@ -5893,10 +5914,10 @@
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C181" s="3">
         <v>3</v>
@@ -5908,7 +5929,7 @@
         <v>2019</v>
       </c>
       <c r="F181" s="3" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="H181" s="4">
         <v>0.43333333333333335</v>
@@ -5920,10 +5941,10 @@
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C182" s="3">
         <v>3</v>
@@ -5935,7 +5956,7 @@
         <v>2019</v>
       </c>
       <c r="F182" s="3" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="H182" s="4">
         <v>0.5</v>
@@ -5947,10 +5968,10 @@
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C183" s="3">
         <v>3</v>
@@ -5962,7 +5983,7 @@
         <v>2019</v>
       </c>
       <c r="F183" s="3" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="H183" s="4">
         <v>0.83333333333333337</v>
@@ -5974,10 +5995,10 @@
     </row>
     <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C184" s="3">
         <v>3</v>
@@ -5989,7 +6010,7 @@
         <v>2019</v>
       </c>
       <c r="F184" s="3" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="H184" s="4">
         <v>0.76666666666666672</v>
@@ -6001,10 +6022,10 @@
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C185" s="3">
         <v>3</v>
@@ -6016,7 +6037,7 @@
         <v>2019</v>
       </c>
       <c r="F185" s="3" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="H185" s="4">
         <v>0.8</v>
@@ -6028,10 +6049,10 @@
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C186" s="3">
         <v>3</v>
@@ -6043,7 +6064,7 @@
         <v>2019</v>
       </c>
       <c r="F186" s="3" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="H186" s="4">
         <v>1</v>
@@ -6055,10 +6076,10 @@
     </row>
     <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C187" s="3">
         <v>3</v>
@@ -6070,7 +6091,7 @@
         <v>2019</v>
       </c>
       <c r="F187" s="3" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="H187" s="4">
         <v>0.8666666666666667</v>
@@ -6082,10 +6103,10 @@
     </row>
     <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C188" s="3">
         <v>3</v>
@@ -6097,7 +6118,7 @@
         <v>2019</v>
       </c>
       <c r="F188" s="3" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="H188" s="4">
         <v>0.6</v>
@@ -6109,10 +6130,10 @@
     </row>
     <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C189" s="3">
         <v>3</v>
@@ -6124,7 +6145,7 @@
         <v>2019</v>
       </c>
       <c r="F189" s="3" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="H189" s="4">
         <v>0.4</v>

</xml_diff>